<commit_message>
Update Outcomes Based on Goals.xlsx
Upload updated workbook
</commit_message>
<xml_diff>
--- a/Outcomes Based on Goals.xlsx
+++ b/Outcomes Based on Goals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julieal-huneidi/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E0733D-3E2C-324B-81AE-0D4212368AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53FB056-9FB3-144A-93C8-7A23D407CCB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="35400" windowHeight="20820" xr2:uid="{357A3EC3-FB14-9340-BAC2-71E50280F933}"/>
   </bookViews>
@@ -1296,7 +1296,7 @@
       <sheetName val="Box Whisker Chart"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="D1" t="str">
@@ -6546,17 +6546,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>